<commit_message>
Tweaked css. Added admob functionality (banner immedietly, interstitial after 30 seconds). Added refresh button and refresh after 5 minutes
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\happyhour_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CBEEB2-CE6A-412C-95C4-E1F88814E2FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08189EF-C0E1-4DCD-B49E-D96F6A80B1BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1931,15 +1931,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BI105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BI2" sqref="BI2:BI105"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="38" width="6" customWidth="1"/>
+    <col min="4" max="36" width="6" customWidth="1"/>
+    <col min="37" max="37" width="10.81640625" customWidth="1"/>
+    <col min="38" max="38" width="6" customWidth="1"/>
     <col min="39" max="39" width="8.54296875" customWidth="1"/>
     <col min="40" max="43" width="6" customWidth="1"/>
     <col min="50" max="50" width="90.54296875" bestFit="1" customWidth="1"/>
@@ -2223,31 +2225,31 @@
         <v>18</v>
       </c>
       <c r="AK2" t="str">
-        <f>IF(H2&gt;0,CONCATENATE(IF(H2&gt;1200,H2/100-12,H2/100),IF(H2&gt;1200,"pm","am"),"-",IF(I2&gt;1200,I2/100-12,I2/100),IF(I2&gt;1200,"pm","am")),"")</f>
+        <f>IF(H2&gt;0,CONCATENATE(IF(H2&gt;=1200,H2/100-12,H2/100),IF(H2&gt;=1200,"pm","am"),"-",IF(I2&gt;=1200,I2/100-12,I2/100),IF(I2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AL2" t="str">
-        <f>IF(J2&gt;0,CONCATENATE(IF(J2&gt;1200,J2/100-12,J2/100),IF(J2&gt;1200,"pm","am"),"-",IF(K2&gt;1200,K2/100-12,K2/100),IF(K2&gt;1200,"pm","am")),"")</f>
+        <f>IF(J2&gt;0,CONCATENATE(IF(J2&gt;=1200,J2/100-12,J2/100),IF(J2&gt;=1200,"pm","am"),"-",IF(K2&gt;=1200,K2/100-12,K2/100),IF(K2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AM2" t="str">
-        <f>IF(L2&gt;0,CONCATENATE(IF(L2&gt;1200,L2/100-12,L2/100),IF(L2&gt;1200,"pm","am"),"-",IF(M2&gt;1200,M2/100-12,M2/100),IF(M2&gt;1200,"pm","am")),"")</f>
+        <f>IF(L2&gt;0,CONCATENATE(IF(L2&gt;=1200,L2/100-12,L2/100),IF(L2&gt;=1200,"pm","am"),"-",IF(M2&gt;=1200,M2/100-12,M2/100),IF(M2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AN2" t="str">
-        <f>IF(N2&gt;0,CONCATENATE(IF(N2&gt;1200,N2/100-12,N2/100),IF(N2&gt;1200,"pm","am"),"-",IF(O2&gt;1200,O2/100-12,O2/100),IF(O2&gt;1200,"pm","am")),"")</f>
+        <f>IF(N2&gt;0,CONCATENATE(IF(N2&gt;=1200,N2/100-12,N2/100),IF(N2&gt;=1200,"pm","am"),"-",IF(O2&gt;=1200,O2/100-12,O2/100),IF(O2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AO2" t="str">
-        <f>IF(P2&gt;0,CONCATENATE(IF(P2&gt;1200,P2/100-12,P2/100),IF(P2&gt;1200,"pm","am"),"-",IF(Q2&gt;1200,Q2/100-12,Q2/100),IF(Q2&gt;1200,"pm","am")),"")</f>
+        <f>IF(P2&gt;0,CONCATENATE(IF(P2&gt;=1200,P2/100-12,P2/100),IF(P2&gt;=1200,"pm","am"),"-",IF(Q2&gt;=1200,Q2/100-12,Q2/100),IF(Q2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AP2" t="str">
-        <f>IF(R2&gt;0,CONCATENATE(IF(R2&gt;1200,R2/100-12,R2/100),IF(R2&gt;1200,"pm","am"),"-",IF(S2&gt;1200,S2/100-12,S2/100),IF(S2&gt;1200,"pm","am")),"")</f>
+        <f>IF(R2&gt;0,CONCATENATE(IF(R2&gt;=1200,R2/100-12,R2/100),IF(R2&gt;=1200,"pm","am"),"-",IF(S2&gt;=1200,S2/100-12,S2/100),IF(S2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AQ2" t="str">
-        <f>IF(T2&gt;0,CONCATENATE(IF(T2&gt;1200,T2/100-12,T2/100),IF(T2&gt;1200,"pm","am"),"-",IF(U2&gt;1200,U2/100-12,U2/100),IF(U2&gt;1200,"pm","am")),"")</f>
+        <f>IF(T2&gt;0,CONCATENATE(IF(T2&gt;=1200,T2/100-12,T2/100),IF(T2&gt;=1200,"pm","am"),"-",IF(U2&gt;=1200,U2/100-12,U2/100),IF(U2&gt;=1200,"pm","am")),"")</f>
         <v>4pm-6pm</v>
       </c>
       <c r="AR2" s="3" t="s">
@@ -2389,31 +2391,31 @@
         <v/>
       </c>
       <c r="AK3" t="str">
-        <f t="shared" ref="AK3:AK66" si="16">IF(H3&gt;0,CONCATENATE(IF(H3&gt;1200,H3/100-12,H3/100),IF(H3&gt;1200,"pm","am"),"-",IF(I3&gt;1200,I3/100-12,I3/100),IF(I3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AK3:AK66" si="16">IF(H3&gt;0,CONCATENATE(IF(H3&gt;=1200,H3/100-12,H3/100),IF(H3&gt;=1200,"pm","am"),"-",IF(I3&gt;=1200,I3/100-12,I3/100),IF(I3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AL3" t="str">
-        <f t="shared" ref="AL3:AL66" si="17">IF(J3&gt;0,CONCATENATE(IF(J3&gt;1200,J3/100-12,J3/100),IF(J3&gt;1200,"pm","am"),"-",IF(K3&gt;1200,K3/100-12,K3/100),IF(K3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AL3:AL66" si="17">IF(J3&gt;0,CONCATENATE(IF(J3&gt;=1200,J3/100-12,J3/100),IF(J3&gt;=1200,"pm","am"),"-",IF(K3&gt;=1200,K3/100-12,K3/100),IF(K3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AM3" t="str">
-        <f t="shared" ref="AM3:AM66" si="18">IF(L3&gt;0,CONCATENATE(IF(L3&gt;1200,L3/100-12,L3/100),IF(L3&gt;1200,"pm","am"),"-",IF(M3&gt;1200,M3/100-12,M3/100),IF(M3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AM3:AM66" si="18">IF(L3&gt;0,CONCATENATE(IF(L3&gt;=1200,L3/100-12,L3/100),IF(L3&gt;=1200,"pm","am"),"-",IF(M3&gt;=1200,M3/100-12,M3/100),IF(M3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AN3" t="str">
-        <f t="shared" ref="AN3:AN66" si="19">IF(N3&gt;0,CONCATENATE(IF(N3&gt;1200,N3/100-12,N3/100),IF(N3&gt;1200,"pm","am"),"-",IF(O3&gt;1200,O3/100-12,O3/100),IF(O3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AN3:AN66" si="19">IF(N3&gt;0,CONCATENATE(IF(N3&gt;=1200,N3/100-12,N3/100),IF(N3&gt;=1200,"pm","am"),"-",IF(O3&gt;=1200,O3/100-12,O3/100),IF(O3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AO3" t="str">
-        <f t="shared" ref="AO3:AO66" si="20">IF(P3&gt;0,CONCATENATE(IF(P3&gt;1200,P3/100-12,P3/100),IF(P3&gt;1200,"pm","am"),"-",IF(Q3&gt;1200,Q3/100-12,Q3/100),IF(Q3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AO3:AO66" si="20">IF(P3&gt;0,CONCATENATE(IF(P3&gt;=1200,P3/100-12,P3/100),IF(P3&gt;=1200,"pm","am"),"-",IF(Q3&gt;=1200,Q3/100-12,Q3/100),IF(Q3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AP3" t="str">
-        <f t="shared" ref="AP3:AP66" si="21">IF(R3&gt;0,CONCATENATE(IF(R3&gt;1200,R3/100-12,R3/100),IF(R3&gt;1200,"pm","am"),"-",IF(S3&gt;1200,S3/100-12,S3/100),IF(S3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AP3:AP66" si="21">IF(R3&gt;0,CONCATENATE(IF(R3&gt;=1200,R3/100-12,R3/100),IF(R3&gt;=1200,"pm","am"),"-",IF(S3&gt;=1200,S3/100-12,S3/100),IF(S3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AQ3" t="str">
-        <f t="shared" ref="AQ3:AQ66" si="22">IF(T3&gt;0,CONCATENATE(IF(T3&gt;1200,T3/100-12,T3/100),IF(T3&gt;1200,"pm","am"),"-",IF(U3&gt;1200,U3/100-12,U3/100),IF(U3&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AQ3:AQ66" si="22">IF(T3&gt;0,CONCATENATE(IF(T3&gt;=1200,T3/100-12,T3/100),IF(T3&gt;=1200,"pm","am"),"-",IF(U3&gt;=1200,U3/100-12,U3/100),IF(U3&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AR3" s="2" t="s">
@@ -6188,7 +6190,7 @@
       </c>
       <c r="AN23" t="str">
         <f t="shared" si="19"/>
-        <v>12am-8pm</v>
+        <v>0pm-8pm</v>
       </c>
       <c r="AO23" t="str">
         <f t="shared" si="20"/>
@@ -6630,7 +6632,7 @@
         <v>[40.587391,-105.075629],</v>
       </c>
     </row>
-    <row r="26" spans="2:61" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:61" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>156</v>
       </c>
@@ -6725,7 +6727,7 @@
       </c>
       <c r="AK26" t="str">
         <f t="shared" si="16"/>
-        <v>12am-7pm</v>
+        <v>0pm-7pm</v>
       </c>
       <c r="AL26" t="str">
         <f t="shared" si="17"/>
@@ -6816,7 +6818,7 @@
         <v>[40.589994,-105.076655],</v>
       </c>
     </row>
-    <row r="27" spans="2:61" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:61" ht="145" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>77</v>
       </c>
@@ -12150,7 +12152,7 @@
         <v>[40.54055,-105.076428],</v>
       </c>
     </row>
-    <row r="56" spans="2:61" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:61" ht="174" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>200</v>
       </c>
@@ -14285,31 +14287,31 @@
         <v/>
       </c>
       <c r="AK67" t="str">
-        <f t="shared" ref="AK67:AK105" si="47">IF(H67&gt;0,CONCATENATE(IF(H67&gt;1200,H67/100-12,H67/100),IF(H67&gt;1200,"pm","am"),"-",IF(I67&gt;1200,I67/100-12,I67/100),IF(I67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AK67:AK105" si="47">IF(H67&gt;0,CONCATENATE(IF(H67&gt;=1200,H67/100-12,H67/100),IF(H67&gt;=1200,"pm","am"),"-",IF(I67&gt;=1200,I67/100-12,I67/100),IF(I67&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AL67" t="str">
-        <f t="shared" ref="AL67:AL105" si="48">IF(J67&gt;0,CONCATENATE(IF(J67&gt;1200,J67/100-12,J67/100),IF(J67&gt;1200,"pm","am"),"-",IF(K67&gt;1200,K67/100-12,K67/100),IF(K67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AL67:AL105" si="48">IF(J67&gt;0,CONCATENATE(IF(J67&gt;=1200,J67/100-12,J67/100),IF(J67&gt;=1200,"pm","am"),"-",IF(K67&gt;=1200,K67/100-12,K67/100),IF(K67&gt;=1200,"pm","am")),"")</f>
         <v>3.3pm-6pm</v>
       </c>
       <c r="AM67" t="str">
-        <f t="shared" ref="AM67:AM105" si="49">IF(L67&gt;0,CONCATENATE(IF(L67&gt;1200,L67/100-12,L67/100),IF(L67&gt;1200,"pm","am"),"-",IF(M67&gt;1200,M67/100-12,M67/100),IF(M67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AM67:AM105" si="49">IF(L67&gt;0,CONCATENATE(IF(L67&gt;=1200,L67/100-12,L67/100),IF(L67&gt;=1200,"pm","am"),"-",IF(M67&gt;=1200,M67/100-12,M67/100),IF(M67&gt;=1200,"pm","am")),"")</f>
         <v>3.3pm-6pm</v>
       </c>
       <c r="AN67" t="str">
-        <f t="shared" ref="AN67:AN105" si="50">IF(N67&gt;0,CONCATENATE(IF(N67&gt;1200,N67/100-12,N67/100),IF(N67&gt;1200,"pm","am"),"-",IF(O67&gt;1200,O67/100-12,O67/100),IF(O67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AN67:AN105" si="50">IF(N67&gt;0,CONCATENATE(IF(N67&gt;=1200,N67/100-12,N67/100),IF(N67&gt;=1200,"pm","am"),"-",IF(O67&gt;=1200,O67/100-12,O67/100),IF(O67&gt;=1200,"pm","am")),"")</f>
         <v>3.3pm-6pm</v>
       </c>
       <c r="AO67" t="str">
-        <f t="shared" ref="AO67:AO105" si="51">IF(P67&gt;0,CONCATENATE(IF(P67&gt;1200,P67/100-12,P67/100),IF(P67&gt;1200,"pm","am"),"-",IF(Q67&gt;1200,Q67/100-12,Q67/100),IF(Q67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AO67:AO105" si="51">IF(P67&gt;0,CONCATENATE(IF(P67&gt;=1200,P67/100-12,P67/100),IF(P67&gt;=1200,"pm","am"),"-",IF(Q67&gt;=1200,Q67/100-12,Q67/100),IF(Q67&gt;=1200,"pm","am")),"")</f>
         <v>3.3pm-6pm</v>
       </c>
       <c r="AP67" t="str">
-        <f t="shared" ref="AP67:AP105" si="52">IF(R67&gt;0,CONCATENATE(IF(R67&gt;1200,R67/100-12,R67/100),IF(R67&gt;1200,"pm","am"),"-",IF(S67&gt;1200,S67/100-12,S67/100),IF(S67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AP67:AP105" si="52">IF(R67&gt;0,CONCATENATE(IF(R67&gt;=1200,R67/100-12,R67/100),IF(R67&gt;=1200,"pm","am"),"-",IF(S67&gt;=1200,S67/100-12,S67/100),IF(S67&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AQ67" t="str">
-        <f t="shared" ref="AQ67:AQ105" si="53">IF(T67&gt;0,CONCATENATE(IF(T67&gt;1200,T67/100-12,T67/100),IF(T67&gt;1200,"pm","am"),"-",IF(U67&gt;1200,U67/100-12,U67/100),IF(U67&gt;1200,"pm","am")),"")</f>
+        <f t="shared" ref="AQ67:AQ105" si="53">IF(T67&gt;0,CONCATENATE(IF(T67&gt;=1200,T67/100-12,T67/100),IF(T67&gt;=1200,"pm","am"),"-",IF(U67&gt;=1200,U67/100-12,U67/100),IF(U67&gt;=1200,"pm","am")),"")</f>
         <v/>
       </c>
       <c r="AR67" s="2" t="s">
@@ -16342,7 +16344,7 @@
         <v>[40.590139,-105.075401],</v>
       </c>
     </row>
-    <row r="79" spans="2:61" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:61" ht="116" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>216</v>
       </c>
@@ -17038,7 +17040,7 @@
         <v>[40.589929,-105.058724],</v>
       </c>
     </row>
-    <row r="83" spans="2:61" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:61" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>325</v>
       </c>
@@ -20797,7 +20799,7 @@
         <v>[40.590724,-105.073266],</v>
       </c>
     </row>
-    <row r="104" spans="2:61" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:61" ht="116" x14ac:dyDescent="0.35">
       <c r="B104" s="10" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Added logical for kids deals
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\happyhour_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A290AC-E8F6-4D0F-932A-5CE358D3EE5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42BDCE2-140F-4023-B07D-64251B0D92F6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2089,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK8" zoomScale="43" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BE2" sqref="BE2:BE118"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="43" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2:AL118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2100,9 +2100,10 @@
     <col min="22" max="22" width="6" style="13" customWidth="1"/>
     <col min="23" max="36" width="6" customWidth="1"/>
     <col min="37" max="37" width="10.81640625" customWidth="1"/>
-    <col min="38" max="38" width="6" customWidth="1"/>
-    <col min="39" max="39" width="8.54296875" customWidth="1"/>
-    <col min="40" max="43" width="6" customWidth="1"/>
+    <col min="38" max="38" width="13.6328125" customWidth="1"/>
+    <col min="39" max="39" width="13" customWidth="1"/>
+    <col min="40" max="42" width="10.26953125" customWidth="1"/>
+    <col min="43" max="43" width="15.90625" customWidth="1"/>
     <col min="50" max="50" width="90.54296875" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10.08984375" customWidth="1"/>
@@ -2393,8 +2394,8 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AL2" t="str">
-        <f>IF(J2&gt;0,CONCATENATE(IF(Y2&lt;=12,Y2,Y2-12),IF(OR(Y2&lt;12,Y2=24),"am","pm"),"-",IF(Z2&lt;=12,Z2,Z2-12),IF(OR(Z2&gt;12,Z2=24),"am","pm")),"")</f>
-        <v>4pm-6am</v>
+        <f>IF(J2&gt;0,CONCATENATE(IF(Y2&lt;=12,Y2,Y2-12),IF(OR(Y2&lt;12,Y2=24),"am","pm"),"-",IF(Z2&lt;=12,Z2,Z2-12),IF(OR(Z2&lt;12,Z2=24),"am","pm")),"")</f>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM2" t="str">
         <f>IF(L2&gt;0,CONCATENATE(IF(AA2&lt;=12,AA2,AA2-12),IF(OR(AA2&lt;12,AA2=24),"am","pm"),"-",IF(AB2&lt;=12,AB2,AB2-12),IF(OR(AB2&lt;12,AB2=24),"am","pm")),"")</f>
@@ -2611,8 +2612,8 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AL3" t="str">
-        <f t="shared" ref="AL3:AL66" si="39">IF(J3&gt;0,CONCATENATE(IF(Y3&lt;=12,Y3,Y3-12),IF(OR(Y3&lt;12,Y3=24),"am","pm"),"-",IF(Z3&lt;=12,Z3,Z3-12),IF(OR(Z3&gt;12,Z3=24),"am","pm")),"")</f>
-        <v>4pm-6am</v>
+        <f t="shared" ref="AL3:AL66" si="39">IF(J3&gt;0,CONCATENATE(IF(Y3&lt;=12,Y3,Y3-12),IF(OR(Y3&lt;12,Y3=24),"am","pm"),"-",IF(Z3&lt;=12,Z3,Z3-12),IF(OR(Z3&lt;12,Z3=24),"am","pm")),"")</f>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM3" t="str">
         <f t="shared" ref="AM3:AM66" si="40">IF(L3&gt;0,CONCATENATE(IF(AA3&lt;=12,AA3,AA3-12),IF(OR(AA3&lt;12,AA3=24),"am","pm"),"-",IF(AB3&lt;=12,AB3,AB3-12),IF(OR(AB3&lt;12,AB3=24),"am","pm")),"")</f>
@@ -3161,7 +3162,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM6" t="str">
         <f t="shared" si="40"/>
@@ -3743,7 +3744,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-7am</v>
+        <v>4pm-7pm</v>
       </c>
       <c r="AM9" t="str">
         <f t="shared" si="40"/>
@@ -3957,7 +3958,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM10" t="str">
         <f t="shared" si="40"/>
@@ -4177,7 +4178,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM11" t="str">
         <f t="shared" si="40"/>
@@ -4542,7 +4543,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-7am</v>
+        <v>3pm-7pm</v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="40"/>
@@ -4753,7 +4754,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" si="39"/>
-        <v>11am-4am</v>
+        <v>11am-4pm</v>
       </c>
       <c r="AM14" t="str">
         <f t="shared" si="40"/>
@@ -4967,7 +4968,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="39"/>
-        <v>10am-2am</v>
+        <v>10am-2pm</v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="40"/>
@@ -5172,7 +5173,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM16" t="str">
         <f t="shared" si="40"/>
@@ -6021,7 +6022,7 @@
       </c>
       <c r="AL21" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM21" t="str">
         <f t="shared" si="40"/>
@@ -6229,7 +6230,7 @@
       </c>
       <c r="AL22" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM22" t="str">
         <f t="shared" si="40"/>
@@ -6437,7 +6438,7 @@
       </c>
       <c r="AL23" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM23" t="str">
         <f t="shared" si="40"/>
@@ -7152,7 +7153,7 @@
       </c>
       <c r="AL27" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM27" t="str">
         <f t="shared" si="40"/>
@@ -7559,7 +7560,7 @@
       </c>
       <c r="AL29" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM29" t="str">
         <f t="shared" si="40"/>
@@ -7758,7 +7759,7 @@
       </c>
       <c r="AL30" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM30" t="str">
         <f t="shared" si="40"/>
@@ -8830,7 +8831,7 @@
       </c>
       <c r="AL36" t="str">
         <f t="shared" si="39"/>
-        <v>4.3pm-7am</v>
+        <v>4.3pm-7pm</v>
       </c>
       <c r="AM36" t="str">
         <f t="shared" si="40"/>
@@ -9041,7 +9042,7 @@
       </c>
       <c r="AL37" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM37" t="str">
         <f t="shared" si="40"/>
@@ -9528,7 +9529,7 @@
       </c>
       <c r="AL40" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM40" t="str">
         <f t="shared" si="40"/>
@@ -9905,7 +9906,7 @@
       </c>
       <c r="AL42" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM42" t="str">
         <f t="shared" si="40"/>
@@ -10107,7 +10108,7 @@
       </c>
       <c r="AL43" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM43" t="str">
         <f t="shared" si="40"/>
@@ -10923,7 +10924,7 @@
       </c>
       <c r="AL48" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-7am</v>
+        <v>4pm-7pm</v>
       </c>
       <c r="AM48" t="str">
         <f t="shared" si="40"/>
@@ -11122,7 +11123,7 @@
       </c>
       <c r="AL49" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM49" t="str">
         <f t="shared" si="40"/>
@@ -11674,7 +11675,7 @@
       </c>
       <c r="AL52" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-8am</v>
+        <v>3pm-8pm</v>
       </c>
       <c r="AM52" t="str">
         <f t="shared" si="40"/>
@@ -12164,7 +12165,7 @@
       </c>
       <c r="AL55" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-7am</v>
+        <v>3pm-7pm</v>
       </c>
       <c r="AM55" t="str">
         <f t="shared" si="40"/>
@@ -12381,7 +12382,7 @@
       </c>
       <c r="AL56" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM56" t="str">
         <f t="shared" si="40"/>
@@ -12595,7 +12596,7 @@
       </c>
       <c r="AL57" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6.3am</v>
+        <v>3pm-6.3pm</v>
       </c>
       <c r="AM57" t="str">
         <f t="shared" si="40"/>
@@ -13295,7 +13296,7 @@
       </c>
       <c r="AL61" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM61" t="str">
         <f t="shared" si="40"/>
@@ -13503,7 +13504,7 @@
       </c>
       <c r="AL62" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-7am</v>
+        <v>4pm-7pm</v>
       </c>
       <c r="AM62" t="str">
         <f t="shared" si="40"/>
@@ -13714,7 +13715,7 @@
       </c>
       <c r="AL63" t="str">
         <f t="shared" si="39"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM63" t="str">
         <f t="shared" si="40"/>
@@ -13928,7 +13929,7 @@
       </c>
       <c r="AL64" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-7am</v>
+        <v>3pm-7pm</v>
       </c>
       <c r="AM64" t="str">
         <f t="shared" si="40"/>
@@ -14308,7 +14309,7 @@
       </c>
       <c r="AL66" t="str">
         <f t="shared" si="39"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM66" t="str">
         <f t="shared" si="40"/>
@@ -14477,7 +14478,7 @@
         <v/>
       </c>
       <c r="AL67" t="str">
-        <f t="shared" ref="AL67:AL118" si="97">IF(J67&gt;0,CONCATENATE(IF(Y67&lt;=12,Y67,Y67-12),IF(OR(Y67&lt;12,Y67=24),"am","pm"),"-",IF(Z67&lt;=12,Z67,Z67-12),IF(OR(Z67&gt;12,Z67=24),"am","pm")),"")</f>
+        <f t="shared" ref="AL67:AL118" si="97">IF(J67&gt;0,CONCATENATE(IF(Y67&lt;=12,Y67,Y67-12),IF(OR(Y67&lt;12,Y67=24),"am","pm"),"-",IF(Z67&lt;=12,Z67,Z67-12),IF(OR(Z67&lt;12,Z67=24),"am","pm")),"")</f>
         <v/>
       </c>
       <c r="AM67" t="str">
@@ -15202,7 +15203,7 @@
       </c>
       <c r="AL71" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM71" t="str">
         <f t="shared" si="98"/>
@@ -15416,7 +15417,7 @@
       </c>
       <c r="AL72" t="str">
         <f t="shared" si="97"/>
-        <v>11am-8.3am</v>
+        <v>11am-8.3pm</v>
       </c>
       <c r="AM72" t="str">
         <f t="shared" si="98"/>
@@ -15781,7 +15782,7 @@
       </c>
       <c r="AL74" t="str">
         <f t="shared" si="97"/>
-        <v>3.3pm-6am</v>
+        <v>3.3pm-6pm</v>
       </c>
       <c r="AM74" t="str">
         <f t="shared" si="98"/>
@@ -16615,7 +16616,7 @@
       </c>
       <c r="AL79" t="str">
         <f t="shared" si="97"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM79" t="str">
         <f t="shared" si="98"/>
@@ -16829,7 +16830,7 @@
       </c>
       <c r="AL80" t="str">
         <f t="shared" si="97"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM80" t="str">
         <f t="shared" si="98"/>
@@ -17108,7 +17109,7 @@
       </c>
       <c r="AL82" t="str">
         <f t="shared" si="97"/>
-        <v>am-pm</v>
+        <v>am-am</v>
       </c>
       <c r="AM82" t="str">
         <f t="shared" si="98"/>
@@ -17488,7 +17489,7 @@
       </c>
       <c r="AL84" t="str">
         <f t="shared" si="97"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM84" t="str">
         <f t="shared" si="98"/>
@@ -17684,7 +17685,7 @@
       </c>
       <c r="AL85" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM85" t="str">
         <f t="shared" si="98"/>
@@ -18779,7 +18780,7 @@
       </c>
       <c r="AL92" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM92" t="str">
         <f t="shared" si="98"/>
@@ -19165,7 +19166,7 @@
       </c>
       <c r="AL94" t="str">
         <f t="shared" si="97"/>
-        <v>4pm-6am</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AM94" t="str">
         <f t="shared" si="98"/>
@@ -20059,7 +20060,7 @@
       </c>
       <c r="AL99" t="str">
         <f t="shared" si="97"/>
-        <v>11am-2am</v>
+        <v>11am-2pm</v>
       </c>
       <c r="AM99" t="str">
         <f t="shared" si="98"/>
@@ -20421,7 +20422,7 @@
       </c>
       <c r="AL101" t="str">
         <f t="shared" si="97"/>
-        <v>5pm-6am</v>
+        <v>5pm-6pm</v>
       </c>
       <c r="AM101" t="str">
         <f t="shared" si="98"/>
@@ -21234,7 +21235,7 @@
       </c>
       <c r="AL106" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM106" t="str">
         <f t="shared" si="98"/>
@@ -21433,7 +21434,7 @@
       </c>
       <c r="AL107" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-6am</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AM107" t="str">
         <f t="shared" si="98"/>
@@ -21947,7 +21948,7 @@
       </c>
       <c r="AL110" t="str">
         <f t="shared" si="97"/>
-        <v>10.3am-7am</v>
+        <v>10.3am-7pm</v>
       </c>
       <c r="AM110" t="str">
         <f t="shared" si="98"/>
@@ -22149,7 +22150,7 @@
       </c>
       <c r="AL111" t="str">
         <f t="shared" si="97"/>
-        <v>3pm-7am</v>
+        <v>3pm-7pm</v>
       </c>
       <c r="AM111" t="str">
         <f t="shared" si="98"/>

</xml_diff>

<commit_message>
Updated 3 margs to see if text is updating
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\happyhour_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\Happy Hour\happyhour_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6527394-62C5-4218-9F75-9B3704CC720F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1519,9 +1518,6 @@
     <t>$3 select brews &lt;br&gt; $4 wells &lt;br&gt; $5 house wines</t>
   </si>
   <si>
-    <t>Tueday: Up to two kids eat free with adult purchase</t>
-  </si>
-  <si>
     <t>2 for 1 Drink Specials &lt;br&gt; Range of Appetizer Specials &lt;br&gt; Buy 1 Sushi Roll, Get Half Off 2nd Roll</t>
   </si>
   <si>
@@ -1634,12 +1630,15 @@
   </si>
   <si>
     <t>Monday-Sunday 11 am-7 pm: &lt;br&gt; $2 domestics and $6 pitchers &lt;br&gt; $2.50-micros and $8 pitchers &lt;br&gt; $2 wells &lt;br&gt; $2 PBR pints (all day) &lt;br&gt; Monday: &lt;br&gt; Happy Hour All Day &lt;br&gt; Tuesday: &lt;br&gt; 2-for-1 burgers 7pm-11pm &lt;br&gt; $2 select micros 7pm-close &lt;br&gt; Wednesday 7 pm-close: &lt;br&gt; $2.50 New Belgium &lt;br&gt; Thursday 7 pm-close: &lt;br&gt; $2.50 Odell beers &lt;br&gt; $1 tacos 6-11 pm &lt;br&gt; Friday: &lt;br&gt; $6 PBR pitchers and $2.50 Jagermeister &lt;br&gt; Saturday: &lt;br&gt; $4 domestic beer and brat &lt;br&gt; Sunday: &lt;br&gt; $16 wings and pitcher (domestic) &lt;br&gt; $19 wings and pitcher (micro)</t>
+  </si>
+  <si>
+    <t>Tueday: Kids eat free (max 2) with adult purchase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1774,7 +1773,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2086,31 +2085,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P84" zoomScale="43" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V68" sqref="V1:V1048576"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="43" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="21" width="6" customWidth="1"/>
     <col min="22" max="22" width="6" style="13" customWidth="1"/>
     <col min="23" max="36" width="6" customWidth="1"/>
-    <col min="37" max="37" width="10.81640625" customWidth="1"/>
-    <col min="38" max="38" width="13.6328125" customWidth="1"/>
+    <col min="37" max="37" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="13.5703125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
-    <col min="40" max="42" width="10.26953125" customWidth="1"/>
-    <col min="43" max="43" width="15.90625" customWidth="1"/>
-    <col min="50" max="50" width="90.54296875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.08984375" customWidth="1"/>
-    <col min="57" max="57" width="53.54296875" customWidth="1"/>
+    <col min="40" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="15.85546875" customWidth="1"/>
+    <col min="50" max="50" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.140625" customWidth="1"/>
+    <col min="57" max="57" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>470</v>
       </c>
@@ -2490,10 +2489,10 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL2" s="12" t="s">
-        <v>497</v>
+        <v>535</v>
       </c>
     </row>
-    <row r="3" spans="2:64" ht="120.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:64" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>140</v>
       </c>
@@ -2701,7 +2700,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>146</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>149</v>
       </c>
@@ -3039,7 +3038,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>109</v>
       </c>
@@ -3467,7 +3466,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>134</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>1900</v>
       </c>
       <c r="V9" s="13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="24"/>
@@ -3835,7 +3834,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:64" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:64" ht="210" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -3894,7 +3893,7 @@
         <v>1800</v>
       </c>
       <c r="V10" s="13" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="W10">
         <f t="shared" si="24"/>
@@ -4055,7 +4054,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>253</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>2400</v>
       </c>
       <c r="V11" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="W11">
         <f t="shared" si="24"/>
@@ -4266,7 +4265,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>52</v>
       </c>
@@ -4432,7 +4431,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>312</v>
       </c>
@@ -4479,7 +4478,7 @@
         <v>1900</v>
       </c>
       <c r="V13" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="24"/>
@@ -4631,7 +4630,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>151</v>
       </c>
@@ -4690,7 +4689,7 @@
         <v>1600</v>
       </c>
       <c r="V14" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="W14">
         <f t="shared" si="24"/>
@@ -4851,7 +4850,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="15" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:64" ht="180" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>274</v>
       </c>
@@ -4904,7 +4903,7 @@
         <v>1600</v>
       </c>
       <c r="V15" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="24"/>
@@ -5062,7 +5061,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>180</v>
       </c>
@@ -5109,7 +5108,7 @@
         <v>1800</v>
       </c>
       <c r="V16" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="24"/>
@@ -5264,7 +5263,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>275</v>
       </c>
@@ -5299,7 +5298,7 @@
         <v>1800</v>
       </c>
       <c r="V17" s="13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="24"/>
@@ -5448,7 +5447,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>182</v>
       </c>
@@ -5620,7 +5619,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>459</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="20" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>380</v>
       </c>
@@ -5899,7 +5898,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:64" ht="180" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>401</v>
       </c>
@@ -5958,7 +5957,7 @@
         <v>1800</v>
       </c>
       <c r="V21" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="W21">
         <f t="shared" si="46"/>
@@ -6113,7 +6112,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>283</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>2300</v>
       </c>
       <c r="V22" s="13" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="W22">
         <f t="shared" si="46"/>
@@ -6327,7 +6326,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="23" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>282</v>
       </c>
@@ -6374,7 +6373,7 @@
         <v>1800</v>
       </c>
       <c r="V23" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="W23" t="str">
         <f t="shared" si="46"/>
@@ -6529,7 +6528,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>126</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>30</v>
       </c>
@@ -6876,7 +6875,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>153</v>
       </c>
@@ -7042,7 +7041,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -7089,7 +7088,7 @@
         <v>1800</v>
       </c>
       <c r="V27" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="W27" t="str">
         <f t="shared" si="46"/>
@@ -7247,7 +7246,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>156</v>
       </c>
@@ -7282,7 +7281,7 @@
         <v>2100</v>
       </c>
       <c r="V28" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="W28">
         <f t="shared" si="46"/>
@@ -7437,7 +7436,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -7496,7 +7495,7 @@
         <v>2400</v>
       </c>
       <c r="V29" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="W29">
         <f t="shared" si="46"/>
@@ -7651,7 +7650,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>460</v>
       </c>
@@ -7850,7 +7849,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="31" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>461</v>
       </c>
@@ -8016,7 +8015,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="32" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>185</v>
       </c>
@@ -8215,7 +8214,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>86</v>
       </c>
@@ -8381,7 +8380,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>68</v>
       </c>
@@ -8551,7 +8550,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>159</v>
       </c>
@@ -8720,7 +8719,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>277</v>
       </c>
@@ -8767,7 +8766,7 @@
         <v>1900</v>
       </c>
       <c r="V36" s="13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="W36" t="str">
         <f t="shared" si="46"/>
@@ -8919,7 +8918,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:64" ht="160.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:64" ht="181.5" x14ac:dyDescent="0.35">
       <c r="B37" s="10" t="s">
         <v>381</v>
       </c>
@@ -8978,7 +8977,7 @@
         <v>1800</v>
       </c>
       <c r="V37" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="W37">
         <f t="shared" si="46"/>
@@ -9130,7 +9129,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>462</v>
       </c>
@@ -9240,7 +9239,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="39" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>264</v>
       </c>
@@ -9406,7 +9405,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>98</v>
       </c>
@@ -9617,7 +9616,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>73</v>
       </c>
@@ -9783,7 +9782,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>278</v>
       </c>
@@ -9997,7 +9996,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>286</v>
       </c>
@@ -10044,7 +10043,7 @@
         <v>1800</v>
       </c>
       <c r="V43" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="W43" t="str">
         <f t="shared" si="70"/>
@@ -10196,7 +10195,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>190</v>
       </c>
@@ -10362,7 +10361,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>192</v>
       </c>
@@ -10528,7 +10527,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>463</v>
       </c>
@@ -10638,7 +10637,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="47" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>194</v>
       </c>
@@ -10807,7 +10806,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>288</v>
       </c>
@@ -10860,7 +10859,7 @@
         <v>1900</v>
       </c>
       <c r="V48" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="W48" t="str">
         <f t="shared" si="71"/>
@@ -11012,7 +11011,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>393</v>
       </c>
@@ -11059,7 +11058,7 @@
         <v>1800</v>
       </c>
       <c r="V49" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="W49">
         <f t="shared" si="71"/>
@@ -11214,7 +11213,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>196</v>
       </c>
@@ -11386,7 +11385,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>46</v>
       </c>
@@ -11552,7 +11551,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>162</v>
       </c>
@@ -11611,7 +11610,7 @@
         <v>2000</v>
       </c>
       <c r="V52" s="13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="W52">
         <f t="shared" si="71"/>
@@ -11766,7 +11765,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>464</v>
       </c>
@@ -11876,7 +11875,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="54" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>198</v>
       </c>
@@ -12042,7 +12041,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>24</v>
       </c>
@@ -12101,7 +12100,7 @@
         <v>1900</v>
       </c>
       <c r="V55" s="13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="W55">
         <f t="shared" si="72"/>
@@ -12259,7 +12258,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>92</v>
       </c>
@@ -12473,7 +12472,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>33</v>
       </c>
@@ -12532,7 +12531,7 @@
         <v>1830</v>
       </c>
       <c r="V57" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="W57">
         <f t="shared" si="72"/>
@@ -12687,7 +12686,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:64" ht="180" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>115</v>
       </c>
@@ -12704,7 +12703,7 @@
         <v>117</v>
       </c>
       <c r="V58" s="13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="W58" t="str">
         <f t="shared" si="72"/>
@@ -12859,7 +12858,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>131</v>
       </c>
@@ -13025,7 +13024,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>95</v>
       </c>
@@ -13191,7 +13190,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>164</v>
       </c>
@@ -13232,7 +13231,7 @@
         <v>1800</v>
       </c>
       <c r="V61" s="13" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="W61" t="str">
         <f t="shared" si="72"/>
@@ -13387,7 +13386,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>390</v>
       </c>
@@ -13440,7 +13439,7 @@
         <v>1900</v>
       </c>
       <c r="V62" s="13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="W62">
         <f t="shared" si="72"/>
@@ -13592,7 +13591,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:64" ht="174" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:64" ht="195" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>200</v>
       </c>
@@ -13651,7 +13650,7 @@
         <v>1800</v>
       </c>
       <c r="V63" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="W63">
         <f t="shared" si="72"/>
@@ -13806,7 +13805,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:64" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:64" ht="210" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>290</v>
       </c>
@@ -13865,7 +13864,7 @@
         <v>1900</v>
       </c>
       <c r="V64" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="W64">
         <f t="shared" si="72"/>
@@ -14017,7 +14016,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>385</v>
       </c>
@@ -14186,7 +14185,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>293</v>
       </c>
@@ -14245,7 +14244,7 @@
         <v>1800</v>
       </c>
       <c r="V66" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="W66">
         <f t="shared" si="72"/>
@@ -14401,7 +14400,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -14573,7 +14572,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>62</v>
       </c>
@@ -14739,7 +14738,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>201</v>
       </c>
@@ -14905,7 +14904,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>408</v>
       </c>
@@ -15080,7 +15079,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="71" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:64" ht="165" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>121</v>
       </c>
@@ -15139,7 +15138,7 @@
         <v>1800</v>
       </c>
       <c r="V71" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="W71">
         <f t="shared" si="72"/>
@@ -15294,7 +15293,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>168</v>
       </c>
@@ -15353,7 +15352,7 @@
         <v>1900</v>
       </c>
       <c r="V72" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="W72">
         <f t="shared" si="72"/>
@@ -15505,7 +15504,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>203</v>
       </c>
@@ -15677,7 +15676,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>170</v>
       </c>
@@ -15718,7 +15717,7 @@
         <v>1800</v>
       </c>
       <c r="V74" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W74" t="str">
         <f t="shared" si="72"/>
@@ -15879,7 +15878,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="75" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>123</v>
       </c>
@@ -16045,7 +16044,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>205</v>
       </c>
@@ -16217,7 +16216,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>143</v>
       </c>
@@ -16383,7 +16382,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>465</v>
       </c>
@@ -16493,7 +16492,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>89</v>
       </c>
@@ -16707,7 +16706,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>207</v>
       </c>
@@ -16766,7 +16765,7 @@
         <v>1800</v>
       </c>
       <c r="V80" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="W80">
         <f t="shared" si="104"/>
@@ -16918,7 +16917,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>209</v>
       </c>
@@ -17087,7 +17086,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>466</v>
       </c>
@@ -17200,7 +17199,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="83" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>211</v>
       </c>
@@ -17372,7 +17371,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>172</v>
       </c>
@@ -17577,7 +17576,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>43</v>
       </c>
@@ -17776,7 +17775,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>213</v>
       </c>
@@ -17945,7 +17944,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>59</v>
       </c>
@@ -18111,7 +18110,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>467</v>
       </c>
@@ -18221,7 +18220,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="89" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>216</v>
       </c>
@@ -18387,7 +18386,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>495</v>
       </c>
@@ -18497,7 +18496,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="91" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>411</v>
       </c>
@@ -18663,7 +18662,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>392</v>
       </c>
@@ -18716,7 +18715,7 @@
         <v>1800</v>
       </c>
       <c r="V92" s="13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="W92">
         <f t="shared" si="107"/>
@@ -18871,7 +18870,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>219</v>
       </c>
@@ -19043,7 +19042,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>295</v>
       </c>
@@ -19254,7 +19253,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>103</v>
       </c>
@@ -19420,7 +19419,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>137</v>
       </c>
@@ -19592,7 +19591,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="97" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>118</v>
       </c>
@@ -19758,7 +19757,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>40</v>
       </c>
@@ -19937,7 +19936,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="99" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>37</v>
       </c>
@@ -20148,7 +20147,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>389</v>
       </c>
@@ -20314,7 +20313,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="2:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>112</v>
       </c>
@@ -20510,7 +20509,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="2:64" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:64" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>80</v>
       </c>
@@ -20679,7 +20678,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>468</v>
       </c>
@@ -20789,7 +20788,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="104" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>100</v>
       </c>
@@ -20955,7 +20954,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>83</v>
       </c>
@@ -21124,7 +21123,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:64" ht="180" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>221</v>
       </c>
@@ -21171,7 +21170,7 @@
         <v>1800</v>
       </c>
       <c r="V106" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="W106" t="str">
         <f t="shared" si="131"/>
@@ -21323,7 +21322,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>175</v>
       </c>
@@ -21370,7 +21369,7 @@
         <v>1800</v>
       </c>
       <c r="V107" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="W107" t="str">
         <f t="shared" si="131"/>
@@ -21522,7 +21521,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="2:64" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>223</v>
       </c>
@@ -21715,7 +21714,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:64" ht="120" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>469</v>
       </c>
@@ -21825,7 +21824,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="110" spans="2:64" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:64" ht="180" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>225</v>
       </c>
@@ -21884,7 +21883,7 @@
         <v>1900</v>
       </c>
       <c r="V110" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="W110">
         <f t="shared" ref="W110:W118" si="132">IF(H110&gt;0,H110/100,"")</f>
@@ -22039,7 +22038,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="2:64" ht="145" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:64" ht="150" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>394</v>
       </c>
@@ -22086,7 +22085,7 @@
         <v>1900</v>
       </c>
       <c r="V111" s="13" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="W111" t="str">
         <f t="shared" si="132"/>
@@ -22241,7 +22240,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="2:64" ht="116" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:64" ht="135" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>228</v>
       </c>
@@ -22407,7 +22406,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="2:63" ht="203" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:63" ht="225" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>297</v>
       </c>
@@ -22466,7 +22465,7 @@
         <v>1900</v>
       </c>
       <c r="V113" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="W113">
         <f t="shared" si="132"/>
@@ -22618,7 +22617,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="2:63" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:63" ht="135" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>415</v>
       </c>
@@ -22787,7 +22786,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="2:63" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:63" ht="135" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>128</v>
       </c>
@@ -22959,7 +22958,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="2:63" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:63" ht="135" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>230</v>
       </c>
@@ -23125,7 +23124,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="2:63" ht="116" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:63" ht="135" x14ac:dyDescent="0.25">
       <c r="B117" s="9" t="s">
         <v>49</v>
       </c>
@@ -23291,7 +23290,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="2:63" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:63" ht="135" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>232</v>
       </c>
@@ -23468,71 +23467,71 @@
     <sortCondition ref="B2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G84" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="AR25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="AR63" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="AR18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="AR73" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="AR12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="AR6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="AR34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AR20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="AR41" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="AR29" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="AR102" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="AR33" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="AR79" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="AR60" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="AR40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="AR104" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="AR95" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="AR11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="AR7" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="AR101" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="AR58" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="AR97" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="AR71" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="AR115" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="AR59" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="AR8" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="AR55" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="AR4" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="AR5" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="AR26" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="AR28" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="AR35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="AR52" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="AR61" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="AR67" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="AR72" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="AR74" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="AR84" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="AR9" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="AR16" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="AR39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="AR50" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="AR54" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="AR69" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="AR80" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="AR86" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="AR89" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="AR93" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="AR106" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="AR108" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="AR112" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="AR118" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="AR15" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="AR36" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="AR42" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="AR43" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="AR48" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="AR64" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="AR66" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="AR94" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="AR113" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="AR37" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="AR49" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="AR30" r:id="rId65" xr:uid="{4ADD2E53-2EA7-49A0-8576-DCB240F148F0}"/>
+    <hyperlink ref="G84" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524"/>
+    <hyperlink ref="AR25" r:id="rId2"/>
+    <hyperlink ref="AR63" r:id="rId3"/>
+    <hyperlink ref="AR18" r:id="rId4"/>
+    <hyperlink ref="AR73" r:id="rId5"/>
+    <hyperlink ref="AR12" r:id="rId6"/>
+    <hyperlink ref="AR6" r:id="rId7"/>
+    <hyperlink ref="AR34" r:id="rId8"/>
+    <hyperlink ref="AR20" r:id="rId9"/>
+    <hyperlink ref="AR41" r:id="rId10"/>
+    <hyperlink ref="AR29" r:id="rId11"/>
+    <hyperlink ref="AR102" r:id="rId12"/>
+    <hyperlink ref="AR33" r:id="rId13"/>
+    <hyperlink ref="AR79" r:id="rId14"/>
+    <hyperlink ref="AR60" r:id="rId15"/>
+    <hyperlink ref="AR40" r:id="rId16"/>
+    <hyperlink ref="AR104" r:id="rId17"/>
+    <hyperlink ref="AR95" r:id="rId18"/>
+    <hyperlink ref="AR11" r:id="rId19"/>
+    <hyperlink ref="AR7" r:id="rId20"/>
+    <hyperlink ref="AR101" r:id="rId21"/>
+    <hyperlink ref="AR58" r:id="rId22"/>
+    <hyperlink ref="AR97" r:id="rId23"/>
+    <hyperlink ref="AR71" r:id="rId24"/>
+    <hyperlink ref="AR115" r:id="rId25"/>
+    <hyperlink ref="AR59" r:id="rId26"/>
+    <hyperlink ref="AR8" r:id="rId27"/>
+    <hyperlink ref="AR55" r:id="rId28"/>
+    <hyperlink ref="AR4" r:id="rId29"/>
+    <hyperlink ref="AR5" r:id="rId30"/>
+    <hyperlink ref="AR26" r:id="rId31"/>
+    <hyperlink ref="AR28" r:id="rId32"/>
+    <hyperlink ref="AR35" r:id="rId33"/>
+    <hyperlink ref="AR52" r:id="rId34"/>
+    <hyperlink ref="AR61" r:id="rId35"/>
+    <hyperlink ref="AR67" r:id="rId36"/>
+    <hyperlink ref="AR72" r:id="rId37"/>
+    <hyperlink ref="AR74" r:id="rId38"/>
+    <hyperlink ref="AR84" r:id="rId39"/>
+    <hyperlink ref="AR9" r:id="rId40"/>
+    <hyperlink ref="AR16" r:id="rId41"/>
+    <hyperlink ref="AR39" r:id="rId42"/>
+    <hyperlink ref="AR50" r:id="rId43"/>
+    <hyperlink ref="AR54" r:id="rId44"/>
+    <hyperlink ref="AR69" r:id="rId45"/>
+    <hyperlink ref="AR80" r:id="rId46"/>
+    <hyperlink ref="AR86" r:id="rId47"/>
+    <hyperlink ref="AR89" r:id="rId48"/>
+    <hyperlink ref="AR93" r:id="rId49"/>
+    <hyperlink ref="AR106" r:id="rId50"/>
+    <hyperlink ref="AR108" r:id="rId51"/>
+    <hyperlink ref="AR112" r:id="rId52"/>
+    <hyperlink ref="AR118" r:id="rId53"/>
+    <hyperlink ref="AR15" r:id="rId54"/>
+    <hyperlink ref="AR36" r:id="rId55"/>
+    <hyperlink ref="AR42" r:id="rId56"/>
+    <hyperlink ref="AR43" r:id="rId57"/>
+    <hyperlink ref="AR48" r:id="rId58"/>
+    <hyperlink ref="AR64" r:id="rId59"/>
+    <hyperlink ref="AR66" r:id="rId60"/>
+    <hyperlink ref="AR94" r:id="rId61"/>
+    <hyperlink ref="AR113" r:id="rId62"/>
+    <hyperlink ref="AR37" r:id="rId63"/>
+    <hyperlink ref="AR49" r:id="rId64"/>
+    <hyperlink ref="AR30" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId66"/>
@@ -23540,14 +23539,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F22D206-CCC0-4994-AA23-452C2700B36E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>

</xml_diff>